<commit_message>
Added CRUD for Restaurant
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Practise\Vega\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -18,6 +23,101 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+  <si>
+    <t>Restaurant</t>
+  </si>
+  <si>
+    <t>RestaurantId</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>PerPersonAmount</t>
+  </si>
+  <si>
+    <t>IsActive</t>
+  </si>
+  <si>
+    <t>MenuItem</t>
+  </si>
+  <si>
+    <t>MenuItemId</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>MenuCategoryId</t>
+  </si>
+  <si>
+    <t>MenuCategory</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Serves Good Kerala food</t>
+  </si>
+  <si>
+    <t>Veg</t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>Good Starter</t>
+  </si>
+  <si>
+    <t>BreakFast</t>
+  </si>
+  <si>
+    <t>Serve you best energentic breakfast</t>
+  </si>
+  <si>
+    <t>FoodCategory</t>
+  </si>
+  <si>
+    <t>Tandoor Chicken</t>
+  </si>
+  <si>
+    <t>MainCourse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Veg non veg main course </t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Restaurant Owner</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>Restaurant Owner Mapping</t>
+  </si>
+  <si>
+    <t>OwnerId</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
@@ -29,12 +129,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +161,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +445,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>300</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bootstrap chagnes and Menu navbar change
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>